<commit_message>
fix(import): :bug: add major bug fixes
isAdditionalField is a boolean in the db and string in DTOs
</commit_message>
<xml_diff>
--- a/src/system/import/tests/sync.xlsx
+++ b/src/system/import/tests/sync.xlsx
@@ -366,7 +366,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -377,6 +377,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -408,22 +414,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -733,72 +742,72 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="22.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="24.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="22.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="39" max="39" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="40" max="40" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="41" max="41" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="42" max="42" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="43" max="43" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="44" max="44" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="45" max="45" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="46" max="46" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="47" max="47" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="48" max="48" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="49" max="49" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="50" max="50" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="51" max="51" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="52" max="52" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="53" max="53" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="54" max="54" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="55" max="55" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="56" max="56" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="57" max="57" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="58" max="58" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="59" max="59" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="60" max="60" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="61" max="61" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="62" max="62" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="63" max="63" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="64" max="64" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="65" max="65" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="66" max="66" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="22.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="24.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="5" width="22.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="5" width="58.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="5" width="32.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="5" width="55.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="39" max="39" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="40" max="40" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="41" max="41" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="42" max="42" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="43" max="43" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="44" max="44" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="45" max="45" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="46" max="46" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="47" max="47" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="48" max="48" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="49" max="49" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="50" max="50" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="51" max="51" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="52" max="52" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="53" max="53" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="54" max="54" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="55" max="55" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="56" max="56" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="57" max="57" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="58" max="58" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="59" max="59" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="60" max="60" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="61" max="61" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="62" max="62" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="63" max="63" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="64" max="64" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="65" max="65" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="66" max="66" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -1024,7 +1033,7 @@
       <c r="H2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="3">
         <v>982257</v>
       </c>
       <c r="J2" s="1" t="s">
@@ -1172,7 +1181,7 @@
       <c r="H3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="3">
         <v>982257</v>
       </c>
       <c r="J3" s="1" t="s">
@@ -1320,7 +1329,7 @@
       <c r="H4" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="3">
         <v>982257</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -1468,7 +1477,7 @@
       <c r="H5" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="3">
         <v>982257</v>
       </c>
       <c r="J5" s="1" t="s">
@@ -1616,7 +1625,7 @@
       <c r="H6" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="3">
         <v>982257</v>
       </c>
       <c r="J6" s="1" t="s">
@@ -1741,7 +1750,7 @@
         <v>56</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1764,7 +1773,7 @@
       <c r="H7" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="4">
         <v>982258</v>
       </c>
       <c r="J7" s="1" t="s">
@@ -1910,7 +1919,7 @@
       <c r="H8" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="3">
         <v>982258</v>
       </c>
       <c r="J8" s="1" t="s">
@@ -2056,7 +2065,7 @@
       <c r="H9" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="3">
         <v>982259</v>
       </c>
       <c r="J9" s="1" t="s">
@@ -2204,7 +2213,7 @@
       <c r="H10" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="3">
         <v>982259</v>
       </c>
       <c r="J10" s="1" t="s">
@@ -2352,7 +2361,7 @@
       <c r="H11" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="3">
         <v>982259</v>
       </c>
       <c r="J11" s="1" t="s">
@@ -2500,7 +2509,7 @@
       <c r="H12" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="3">
         <v>982259</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -2648,7 +2657,7 @@
       <c r="H13" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="3">
         <v>982259</v>
       </c>
       <c r="J13" s="1" t="s">

</xml_diff>